<commit_message>
fixed errors after KLR16
</commit_message>
<xml_diff>
--- a/Spreadsheets/Latent Defect Estimation.xlsx
+++ b/Spreadsheets/Latent Defect Estimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -340,18 +340,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1840,7 +1840,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2238,29 +2238,29 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="O4" s="11">
+      <c r="O4" s="9">
         <v>1</v>
       </c>
       <c r="P4" t="s">
@@ -2268,16 +2268,16 @@
       </c>
     </row>
     <row r="20" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O20" s="11"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O21" s="11"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O22" s="11"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O23" s="11"/>
+      <c r="O23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2290,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="F10" sqref="F10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2306,21 +2306,21 @@
     <col min="11" max="11" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2468,25 +2468,29 @@
       </c>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="F10" s="4">
+      <c r="F10" s="11">
         <f>IFERROR(CEILING((TotalA*TotalB)/Both,1),"More data  required")</f>
         <v>10</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="K10">
+        <f>4*5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2495,31 +2499,31 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="F13" s="4">
+      <c r="F13" s="11">
         <f>IFERROR(TotalEstimatedDefects-TotalDefects,"More data required")</f>
         <v>3</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3085,38 +3089,38 @@
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>